<commit_message>
Changes to the household script
</commit_message>
<xml_diff>
--- a/model/Livestock_SDMX_Model.xlsx
+++ b/model/Livestock_SDMX_Model.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\rara\RAP\Agriculture\sdd-household-primary-activity-processing\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896F7BF0-0AB0-45FB-9A00-F50252336AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958DD574-FF39-4F3F-A347-6DB264B9CB24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="135" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="DSD" sheetId="1" r:id="rId1"/>
+    <sheet name="DSD_LIVESTOCK" sheetId="1" r:id="rId1"/>
     <sheet name="LIVESTOCK_PIG" sheetId="6" r:id="rId2"/>
     <sheet name="LIVESTOCK_CHICKEN" sheetId="8" r:id="rId3"/>
     <sheet name="LIVESTOCK_DUCK" sheetId="9" r:id="rId4"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="68">
   <si>
     <t>Concepts</t>
   </si>
@@ -217,9 +217,6 @@
     <t>raising other livestock</t>
   </si>
   <si>
-    <t>CL_COM_YESNO</t>
-  </si>
-  <si>
     <t>CL_COM_GEO_PICT_L123</t>
   </si>
   <si>
@@ -236,6 +233,18 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>CL_LIVESTOCK_PIG</t>
+  </si>
+  <si>
+    <t>CL_LIVESTOCK_CHICKEN</t>
+  </si>
+  <si>
+    <t>CL_LIVESTOCK_DUCK</t>
+  </si>
+  <si>
+    <t>CL_LIVESTOCK_OTHER</t>
   </si>
 </sst>
 </file>
@@ -595,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,7 +704,7 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
@@ -718,7 +727,7 @@
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
@@ -787,7 +796,7 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="G8" t="s">
         <v>9</v>
@@ -810,7 +819,7 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -833,7 +842,7 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
@@ -856,7 +865,7 @@
         <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
@@ -985,18 +994,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1037,18 +1046,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1068,7 +1077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A711D74A-BF47-4DF1-A9CD-277DE80B1187}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1089,18 +1098,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1141,18 +1150,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>